<commit_message>
Add workflow to scrape Bergey daily summaries from the web and save the data in this directory.
</commit_message>
<xml_diff>
--- a/notebooks/validation/01 Bergey Turbine Data/bergey_sites.xlsx
+++ b/notebooks/validation/01 Bergey Turbine Data/bergey_sites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cphillip/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cphillip/Projects/dw-tap/notebooks/validation/01 Bergey Turbine Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119F9EA2-B98E-7943-B213-D473BD573563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DB3E17-C1FA-E54E-B9F5-CA50E43E2D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22500" yWindow="1760" windowWidth="27020" windowHeight="26260" xr2:uid="{76F781A1-2517-477F-8E9B-0334CCA2CB5B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="120">
   <si>
     <t>State</t>
   </si>
@@ -336,6 +336,66 @@
   </si>
   <si>
     <t>t221</t>
+  </si>
+  <si>
+    <t>A2719</t>
+  </si>
+  <si>
+    <t>A2672</t>
+  </si>
+  <si>
+    <t>A3479</t>
+  </si>
+  <si>
+    <t>A2715</t>
+  </si>
+  <si>
+    <t>A2272</t>
+  </si>
+  <si>
+    <t>A3031</t>
+  </si>
+  <si>
+    <t>A2734</t>
+  </si>
+  <si>
+    <t>A2690</t>
+  </si>
+  <si>
+    <t>A2275</t>
+  </si>
+  <si>
+    <t>A3898</t>
+  </si>
+  <si>
+    <t>A3498</t>
+  </si>
+  <si>
+    <t>A3835</t>
+  </si>
+  <si>
+    <t>A3679</t>
+  </si>
+  <si>
+    <t>A3933</t>
+  </si>
+  <si>
+    <t>A2744</t>
+  </si>
+  <si>
+    <t>A3685</t>
+  </si>
+  <si>
+    <t>A2723</t>
+  </si>
+  <si>
+    <t>A2271</t>
+  </si>
+  <si>
+    <t>A2671</t>
+  </si>
+  <si>
+    <t>AID</t>
   </si>
 </sst>
 </file>
@@ -708,645 +768,706 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEBD7D1-F9F5-4443-8FB7-B1FE46FED9F0}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="2"/>
-    <col min="2" max="2" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.83203125" style="2"/>
-    <col min="7" max="7" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="50.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="2"/>
-    <col min="11" max="11" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="14.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8.83203125" style="2"/>
+    <col min="8" max="8" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="50.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="2"/>
+    <col min="12" max="12" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>43.918621999999999</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>-91.899497999999994</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>41</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>39.331088000000001</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>-119.820234</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>30</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>40.851353000000003</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>-75.598394999999996</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>30</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>43.524158</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>-76.372290000000007</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>31</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>43.463999999999999</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>-76.510999999999996</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>43.047418</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>-92.981673999999998</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>37</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>45.57217</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>-96.034237000000005</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>37</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>34.519542000000001</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>-120.081227</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>24</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>37.857793999999998</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>-84.712430999999995</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>43</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>39.328563000000003</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>-89.402379999999994</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>37</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>44.286304999999999</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>-105.335035</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>24</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>42.600527999999997</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>-94.972624999999994</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>31</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>40.979106999999999</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>-72.136609000000007</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>37</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>40.870730999999999</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>-72.888835</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>41.076813000000001</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>-85.116973999999999</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>37</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>42.166797000000003</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>-84.403169000000005</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>24</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>44.192568999999999</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>-75.964894999999999</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>37</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>39.417489000000003</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>-88.387005000000002</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>27</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>44.987588000000002</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>-72.072199999999995</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>43</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>41.48359</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>-87.723669000000001</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>37</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <v>42.510050999999997</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>-92.457859999999997</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>30</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M20">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N20">
     <sortCondition ref="A2:A20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add metadata about lidar availability for all 19 sites
</commit_message>
<xml_diff>
--- a/notebooks/validation/01 Bergey Turbine Data/bergey_sites.xlsx
+++ b/notebooks/validation/01 Bergey Turbine Data/bergey_sites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cphillip/Projects/dw-tap/notebooks/validation/01 Bergey Turbine Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DB3E17-C1FA-E54E-B9F5-CA50E43E2D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13E30A8-7EAD-5844-8695-D62F79C0A14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22500" yWindow="1760" windowWidth="27020" windowHeight="26260" xr2:uid="{76F781A1-2517-477F-8E9B-0334CCA2CB5B}"/>
+    <workbookView xWindow="1440" yWindow="8420" windowWidth="30240" windowHeight="18880" xr2:uid="{76F781A1-2517-477F-8E9B-0334CCA2CB5B}"/>
   </bookViews>
   <sheets>
     <sheet name="APRS World" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="171">
   <si>
     <t>State</t>
   </si>
@@ -396,6 +396,159 @@
   </si>
   <si>
     <t>AID</t>
+  </si>
+  <si>
+    <t>QL1/QL3</t>
+  </si>
+  <si>
+    <t>QL2</t>
+  </si>
+  <si>
+    <t>Lidar Quality</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/IA_Statewide_2008</t>
+  </si>
+  <si>
+    <t>LPC Link</t>
+  </si>
+  <si>
+    <t>Raster DEM Link</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/IL_4_County_QL1_LiDAR_2016_B16/IL_4County_Cook_2017</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/USGS_LPC_IL_4County_Cook_2017_LAS_2019</t>
+  </si>
+  <si>
+    <t>Urban/Suburban</t>
+  </si>
+  <si>
+    <t>Building Data Quality</t>
+  </si>
+  <si>
+    <t>Site Type</t>
+  </si>
+  <si>
+    <t>Poor, most missing</t>
+  </si>
+  <si>
+    <t>Good coverage</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/Eastern_Vermont_LiDAR_FY2014/VT_EasternVermont_L1_2014</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/USGS_LPC_VT_EasternVermont_L1_2014_LAS_2017</t>
+  </si>
+  <si>
+    <t>Partial, some missing</t>
+  </si>
+  <si>
+    <t>QL3</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/Contributed_ILDOT_District_7_QL3/IL_District7_Coles_2014</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/__IL_District7-Coles_2014/</t>
+  </si>
+  <si>
+    <t>Rural/Suburban</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/USGS_LPC_NY_GreatLakes_Phase2_L3_2014_LAS_2017</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/FEMA_Region_2_NY_Great_Lakes_Area_QL2_LiDAR/NY_GreatLakes_Phase2_L3_2014</t>
+  </si>
+  <si>
+    <t>Suburban</t>
+  </si>
+  <si>
+    <t>Good, few missing</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/legacy/MI_LAKEERIE_UTM16_2010</t>
+  </si>
+  <si>
+    <t>QL2/QL3</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/IN_Indiana_Statewide_LiDAR_2017_B17/IN_Statewide_B2_2017</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/IN_Indiana_Statewide_LiDAR_2017_B17/IN_Statewide_B2_2017</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/Long_Island_NY_SANDY_LiDAR/NY_LongIsland_Z18_2014</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/Long_Island_NY_SANDY_LiDAR/NY_LongIsland-Z18_2014</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/IA_NorthCentral_2020_D20/IA_NorthCentral_3_2020</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/IA_NorthCentral_2020_D20/IA_NorthCentral_3_2020</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/WY_North_Converse_2020_D20/WY_NConverse_2_2020</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/WY_North_Converse_2020_D20/WY_NConverse_2_2020</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/USGS_LPC_IL_GrnMacMont_2017_LAS_2018</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/IL_GreenMacoupinMont_2017_C18/IL_GrnMacMont_2017</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/KY_Eastern_2019_A19/KY_Eastern_B1_2019</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/KY_Eastern_2019_A19/KY_Eastern_B1_2019</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/CA_SoCAL_Wildfires_2018_D18/CA_SoCal_Wildfires_B4_2018</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/CA_SoCAL_Wildfires_2018_D18/CA_SoCal_Wildfires_B4_2018</t>
+  </si>
+  <si>
+    <t>N/A (Legacy Data)</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/IWI_RedRiver-DL_2009</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/USGS_LPC_NY_CayugaOswego_2018_LAS_2019</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/NY_CayugaOswegoCounties_2018_A18/NY_CayugaOswego_2018</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/PA_Northcentral_2019_B19/PA_Northcentral_B5_2019</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/PA_Northcentral_2019_B19/PA_Northcentral_B5_2019</t>
+  </si>
+  <si>
+    <t>QL1</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/USGS_LPC_NV_Reno_Carson_QL1_2017_LAS_2018</t>
+  </si>
+  <si>
+    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/NV_Reno_Carson_Urban_Lidar_2017_B17/NV_Reno_Carson_QL1_2017</t>
+  </si>
+  <si>
+    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/MN_SEMN_2008</t>
   </si>
 </sst>
 </file>
@@ -768,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEBD7D1-F9F5-4443-8FB7-B1FE46FED9F0}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -782,15 +935,17 @@
     <col min="4" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="8.83203125" style="2"/>
     <col min="8" max="8" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="50.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="2"/>
-    <col min="12" max="12" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="2"/>
+    <col min="9" max="12" width="11.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.83203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="50.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" style="2"/>
+    <col min="17" max="17" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
@@ -816,25 +971,40 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
@@ -860,13 +1030,25 @@
         <v>41</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>88</v>
       </c>
@@ -892,13 +1074,28 @@
         <v>30</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>82</v>
       </c>
@@ -924,13 +1121,28 @@
         <v>30</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>95</v>
       </c>
@@ -956,25 +1168,40 @@
         <v>31</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L5" s="2">
+      <c r="Q5" s="2">
         <v>43.463999999999999</v>
       </c>
-      <c r="M5" s="2">
+      <c r="R5" s="2">
         <v>-76.510999999999996</v>
       </c>
-      <c r="N5" s="2">
+      <c r="S5" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>93</v>
       </c>
@@ -1000,13 +1227,25 @@
         <v>37</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>86</v>
       </c>
@@ -1032,13 +1271,25 @@
         <v>37</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>98</v>
       </c>
@@ -1064,13 +1315,28 @@
         <v>24</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>85</v>
       </c>
@@ -1096,13 +1362,28 @@
         <v>43</v>
       </c>
       <c r="I9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>97</v>
       </c>
@@ -1128,13 +1409,28 @@
         <v>37</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>87</v>
       </c>
@@ -1160,13 +1456,28 @@
         <v>24</v>
       </c>
       <c r="I11" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>89</v>
       </c>
@@ -1192,13 +1503,28 @@
         <v>31</v>
       </c>
       <c r="I12" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>92</v>
       </c>
@@ -1224,25 +1550,40 @@
         <v>37</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="L13" s="2">
+      <c r="Q13" s="2">
         <v>40.870730999999999</v>
       </c>
-      <c r="M13" s="2">
+      <c r="R13" s="2">
         <v>-72.888835</v>
       </c>
-      <c r="N13" s="2">
+      <c r="S13" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>91</v>
       </c>
@@ -1268,13 +1609,28 @@
         <v>37</v>
       </c>
       <c r="I14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>84</v>
       </c>
@@ -1300,13 +1656,25 @@
         <v>24</v>
       </c>
       <c r="I15" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>90</v>
       </c>
@@ -1332,13 +1700,28 @@
         <v>37</v>
       </c>
       <c r="I16" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="N16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>81</v>
       </c>
@@ -1364,13 +1747,28 @@
         <v>27</v>
       </c>
       <c r="I17" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>83</v>
       </c>
@@ -1396,13 +1794,28 @@
         <v>43</v>
       </c>
       <c r="I18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="N18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="O18" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>96</v>
       </c>
@@ -1428,13 +1841,28 @@
         <v>37</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="O19" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
@@ -1460,14 +1888,26 @@
         <v>30</v>
       </c>
       <c r="I20" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="O20" s="2" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N20">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S20">
     <sortCondition ref="A2:A20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated site spreadsheet and bias correction datafiles from Lindsay
</commit_message>
<xml_diff>
--- a/notebooks/validation/01 Bergey Turbine Data/bergey_sites.xlsx
+++ b/notebooks/validation/01 Bergey Turbine Data/bergey_sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cphillip/Projects/dw-tap/notebooks/validation/01 Bergey Turbine Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13E30A8-7EAD-5844-8695-D62F79C0A14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{96E0308D-A62C-5749-A36F-70DA344480DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="8420" windowWidth="30240" windowHeight="18880" xr2:uid="{76F781A1-2517-477F-8E9B-0334CCA2CB5B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="164">
   <si>
     <t>State</t>
   </si>
@@ -272,12 +272,6 @@
     <t>Measurement Height (m)</t>
   </si>
   <si>
-    <t>Oswego</t>
-  </si>
-  <si>
-    <t>Brookhaven</t>
-  </si>
-  <si>
     <t>APRS ID</t>
   </si>
   <si>
@@ -398,30 +392,12 @@
     <t>AID</t>
   </si>
   <si>
-    <t>QL1/QL3</t>
-  </si>
-  <si>
     <t>QL2</t>
   </si>
   <si>
     <t>Lidar Quality</t>
   </si>
   <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/IA_Statewide_2008</t>
-  </si>
-  <si>
-    <t>LPC Link</t>
-  </si>
-  <si>
-    <t>Raster DEM Link</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/IL_4_County_QL1_LiDAR_2016_B16/IL_4County_Cook_2017</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/USGS_LPC_IL_4County_Cook_2017_LAS_2019</t>
-  </si>
-  <si>
     <t>Urban/Suburban</t>
   </si>
   <si>
@@ -437,125 +413,128 @@
     <t>Good coverage</t>
   </si>
   <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/Eastern_Vermont_LiDAR_FY2014/VT_EasternVermont_L1_2014</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/USGS_LPC_VT_EasternVermont_L1_2014_LAS_2017</t>
-  </si>
-  <si>
     <t>Partial, some missing</t>
   </si>
   <si>
-    <t>QL3</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/Contributed_ILDOT_District_7_QL3/IL_District7_Coles_2014</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/__IL_District7-Coles_2014/</t>
-  </si>
-  <si>
     <t>Rural/Suburban</t>
   </si>
   <si>
     <t>Rural</t>
   </si>
   <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/USGS_LPC_NY_GreatLakes_Phase2_L3_2014_LAS_2017</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/FEMA_Region_2_NY_Great_Lakes_Area_QL2_LiDAR/NY_GreatLakes_Phase2_L3_2014</t>
-  </si>
-  <si>
     <t>Suburban</t>
   </si>
   <si>
     <t>Good, few missing</t>
   </si>
   <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/legacy/MI_LAKEERIE_UTM16_2010</t>
-  </si>
-  <si>
-    <t>QL2/QL3</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/IN_Indiana_Statewide_LiDAR_2017_B17/IN_Statewide_B2_2017</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/IN_Indiana_Statewide_LiDAR_2017_B17/IN_Statewide_B2_2017</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/Long_Island_NY_SANDY_LiDAR/NY_LongIsland_Z18_2014</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/Long_Island_NY_SANDY_LiDAR/NY_LongIsland-Z18_2014</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/IA_NorthCentral_2020_D20/IA_NorthCentral_3_2020</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/IA_NorthCentral_2020_D20/IA_NorthCentral_3_2020</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/WY_North_Converse_2020_D20/WY_NConverse_2_2020</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/WY_North_Converse_2020_D20/WY_NConverse_2_2020</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/USGS_LPC_IL_GrnMacMont_2017_LAS_2018</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/IL_GreenMacoupinMont_2017_C18/IL_GrnMacMont_2017</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/KY_Eastern_2019_A19/KY_Eastern_B1_2019</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/KY_Eastern_2019_A19/KY_Eastern_B1_2019</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/CA_SoCAL_Wildfires_2018_D18/CA_SoCal_Wildfires_B4_2018</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/CA_SoCAL_Wildfires_2018_D18/CA_SoCal_Wildfires_B4_2018</t>
-  </si>
-  <si>
     <t>N/A (Legacy Data)</t>
   </si>
   <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/IWI_RedRiver-DL_2009</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/USGS_LPC_NY_CayugaOswego_2018_LAS_2019</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/NY_CayugaOswegoCounties_2018_A18/NY_CayugaOswego_2018</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/PA_Northcentral_2019_B19/PA_Northcentral_B5_2019</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/PA_Northcentral_2019_B19/PA_Northcentral_B5_2019</t>
-  </si>
-  <si>
     <t>QL1</t>
   </si>
   <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/USGS_LPC_NV_Reno_Carson_QL1_2017_LAS_2018</t>
-  </si>
-  <si>
-    <t>http://prd-tnm.s3.amazonaws.com/index.html?prefix=StagedProducts/Elevation/OPR/Projects/NV_Reno_Carson_Urban_Lidar_2017_B17/NV_Reno_Carson_QL1_2017</t>
-  </si>
-  <si>
-    <t>https://rockyweb.usgs.gov/vdelivery/Datasets/Staged/Elevation/LPC/Projects/MN_SEMN_2008</t>
+    <t>il_pioneertrail</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>vt_proctormaple</t>
+  </si>
+  <si>
+    <t>oh_toledo</t>
+  </si>
+  <si>
+    <t>ny_brookhaven</t>
+  </si>
+  <si>
+    <t>mn_prairiestar</t>
+  </si>
+  <si>
+    <t>30, 50</t>
+  </si>
+  <si>
+    <t>ny_oswego</t>
+  </si>
+  <si>
+    <t>Measurement Privacy</t>
+  </si>
+  <si>
+    <t>Proprietary</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Site Notes</t>
+  </si>
+  <si>
+    <t>No lidar data. This turbine is absolutely surrounded by trees.</t>
+  </si>
+  <si>
+    <t>Straight forward high desert site outside Reno, but with some mature pine trees. The largest are 11m.</t>
+  </si>
+  <si>
+    <t>Impressive amount of vegetation – some sections completely forested.</t>
+  </si>
+  <si>
+    <t>Lakeshore, heavily forested.</t>
+  </si>
+  <si>
+    <t>Very simple site, one building and a couple small trees. Comparable complexity to the EAZ study. Interestingly It does look like they’ve planted a bunch of trees around the turbine but they are very small right now.</t>
+  </si>
+  <si>
+    <t>No lidar data. One large building to the NE. Impressive hedgerows.</t>
+  </si>
+  <si>
+    <t>This is in the coastal foothills outside Santa Barbara. Obstacle-wise this site is straight forward, but what’s interesting is the sloping terrain.</t>
+  </si>
+  <si>
+    <t>Lidar data only covers about 90% of the 1km radius but appears to cover all the obstacles and the whole 200m radius. Partially forested, turbine is basically boxed in by trees in four directions – should be an interesting site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A rural site in Illinois has a very large silo. Our lidar data estimates that silo at 37m tall. </t>
+  </si>
+  <si>
+    <t>Wyoming junk yard. Very little vegetation.</t>
+  </si>
+  <si>
+    <t>Typical rural site with more vegetation.</t>
+  </si>
+  <si>
+    <t>Second site where a larger 100m turbine appears to be under construction, but only visible in the newest google satellite imagery.</t>
+  </si>
+  <si>
+    <t>Another campus site with many obstacles and many mature trees.</t>
+  </si>
+  <si>
+    <t>Baseball diamonds near lake/wetland bordered by mature trees.</t>
+  </si>
+  <si>
+    <t>Utility-scale turbine being constructed next to the Bergey – this does show up in the lidar data (118m maximum). Historical street-view data suggests it went up sometime between 2018 and 2022, but the blades are not attached in the most recent imagery.</t>
+  </si>
+  <si>
+    <t>Fairly straightforward rural site with relatively few obstacles. Comparable in complexity to EAZ study.</t>
+  </si>
+  <si>
+    <t>Urban. I’m wondering about the influence of the forested area to the SE, and also the large number of buildings -- should be an interesting site.</t>
+  </si>
+  <si>
+    <t>Campus site. The median height doesn’t work well for the trees here, while the maximum seems more reliable.</t>
+  </si>
+  <si>
+    <t>Isolated campus site with sparse vegetation and buildings.</t>
+  </si>
+  <si>
+    <t>Lidar Collection Year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -578,13 +557,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -599,12 +591,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -921,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEBD7D1-F9F5-4443-8FB7-B1FE46FED9F0}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -945,12 +946,12 @@
     <col min="19" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>46</v>
@@ -971,19 +972,19 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>22</v>
@@ -1003,13 +1004,16 @@
       <c r="S1" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="T1" s="1" t="s">
+        <v>140</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>61</v>
@@ -1030,16 +1034,19 @@
         <v>41</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>170</v>
+        <v>133</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>23</v>
@@ -1047,13 +1054,28 @@
       <c r="O2" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="P2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>43.673000000000002</v>
+      </c>
+      <c r="R2" s="3">
+        <v>-92.697999999999993</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>35</v>
@@ -1074,19 +1096,19 @@
         <v>30</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>168</v>
+        <v>131</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2020</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>169</v>
+        <v>126</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>23</v>
@@ -1095,12 +1117,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -1121,19 +1143,19 @@
         <v>30</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>165</v>
+        <v>118</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2019</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>23</v>
@@ -1142,12 +1164,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>64</v>
@@ -1168,19 +1190,19 @@
         <v>31</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>163</v>
+        <v>118</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2018</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>164</v>
+        <v>127</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>23</v>
@@ -1189,7 +1211,7 @@
         <v>63</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
       <c r="Q5" s="2">
         <v>43.463999999999999</v>
@@ -1200,13 +1222,16 @@
       <c r="S5" s="2">
         <v>15</v>
       </c>
+      <c r="T5" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>27</v>
@@ -1227,16 +1252,19 @@
         <v>37</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2020</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>23</v>
@@ -1245,12 +1273,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>30</v>
@@ -1271,16 +1299,19 @@
         <v>37</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>162</v>
+        <v>133</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>23</v>
@@ -1289,12 +1320,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>38</v>
@@ -1315,19 +1346,19 @@
         <v>24</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>159</v>
+        <v>118</v>
+      </c>
+      <c r="J8" s="2">
+        <v>2018</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>23</v>
@@ -1336,12 +1367,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>25</v>
@@ -1362,19 +1393,19 @@
         <v>43</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>157</v>
+        <v>118</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2019</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>23</v>
@@ -1383,12 +1414,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>69</v>
@@ -1409,19 +1440,19 @@
         <v>37</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>155</v>
+        <v>118</v>
+      </c>
+      <c r="J10" s="2">
+        <v>2017</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>23</v>
@@ -1429,13 +1460,28 @@
       <c r="O10" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="P10" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>40.487000000000002</v>
+      </c>
+      <c r="R10" s="3">
+        <v>-88.05</v>
+      </c>
+      <c r="S10" s="3">
+        <v>48</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>33</v>
@@ -1456,19 +1502,19 @@
         <v>24</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J11" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2020</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="M11" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>23</v>
@@ -1477,12 +1523,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>39</v>
@@ -1503,19 +1549,19 @@
         <v>31</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>151</v>
+        <v>118</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2020</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>23</v>
@@ -1524,12 +1570,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
@@ -1550,19 +1596,19 @@
         <v>37</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>149</v>
+        <v>118</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2014</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>56</v>
@@ -1571,7 +1617,7 @@
         <v>58</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="Q13" s="2">
         <v>40.870730999999999</v>
@@ -1582,13 +1628,16 @@
       <c r="S13" s="2">
         <v>50</v>
       </c>
+      <c r="T13" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>45</v>
@@ -1609,19 +1658,19 @@
         <v>37</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>148</v>
+        <v>118</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2017</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>23</v>
@@ -1630,12 +1679,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
@@ -1656,16 +1705,19 @@
         <v>24</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>145</v>
+        <v>118</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2018</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>23</v>
@@ -1673,13 +1725,26 @@
       <c r="O15" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="P15" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>41.694000000000003</v>
+      </c>
+      <c r="R15" s="2">
+        <v>-83.472999999999999</v>
+      </c>
+      <c r="S15" s="2">
+        <v>26</v>
+      </c>
+      <c r="T15" s="5"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>42</v>
@@ -1700,19 +1765,19 @@
         <v>37</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>141</v>
+        <v>118</v>
+      </c>
+      <c r="J16" s="2">
+        <v>2014</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>23</v>
@@ -1720,13 +1785,17 @@
       <c r="O16" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>24</v>
@@ -1747,19 +1816,19 @@
         <v>27</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>137</v>
+        <v>118</v>
+      </c>
+      <c r="J17" s="2">
+        <v>2020</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>23</v>
@@ -1767,13 +1836,28 @@
       <c r="O17" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="P17" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>40.487000000000002</v>
+      </c>
+      <c r="R17" s="3">
+        <v>-88.05</v>
+      </c>
+      <c r="S17" s="3">
+        <v>48</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>19</v>
@@ -1794,19 +1878,19 @@
         <v>43</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>134</v>
+        <v>118</v>
+      </c>
+      <c r="J18" s="2">
+        <v>2014</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>23</v>
@@ -1814,13 +1898,28 @@
       <c r="O18" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="P18" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>44.526470000000003</v>
+      </c>
+      <c r="R18" s="2">
+        <v>-72.866061999999999</v>
+      </c>
+      <c r="S18" s="2">
+        <v>24</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>67</v>
@@ -1841,19 +1940,19 @@
         <v>37</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J19" s="2">
+        <v>2017</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="J19" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="L19" s="2" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>23</v>
@@ -1861,13 +1960,28 @@
       <c r="O19" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="P19" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>40.487000000000002</v>
+      </c>
+      <c r="R19" s="3">
+        <v>-88.05</v>
+      </c>
+      <c r="S19" s="3">
+        <v>48</v>
+      </c>
+      <c r="T19" s="5" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>71</v>
@@ -1888,16 +2002,19 @@
         <v>30</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
+      </c>
+      <c r="J20" s="2">
+        <v>2020</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>128</v>
+        <v>161</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>23</v>
@@ -1905,6 +2022,9 @@
       <c r="O20" s="2" t="s">
         <v>70</v>
       </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="P23" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S20">

</xml_diff>